<commit_message>
update final end poss event results
</commit_message>
<xml_diff>
--- a/Final_End_Poss_Event_Results.xlsx
+++ b/Final_End_Poss_Event_Results.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d4fd6e6c2e864131/Documents/STAT 5713 - Advanced Data Mining/Final Project/predicting-pass-outcome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14DA3819-B143-486E-B7DA-7B27122210B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{14DA3819-B143-486E-B7DA-7B27122210B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76C0D5C9-CC9E-4D62-BDA7-3F95F79B25A3}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{14ABE528-ACF9-44C9-85F4-AB3048AD34F7}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{14ABE528-ACF9-44C9-85F4-AB3048AD34F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Incomplete Play" sheetId="2" r:id="rId1"/>
+    <sheet name="Goal" sheetId="3" r:id="rId2"/>
+    <sheet name="Shot" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goal!$A$1:$H$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incomplete Play'!$A$1:$H$164</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="87">
   <si>
     <t>Previous_Items1</t>
   </si>
@@ -219,6 +222,87 @@
   </si>
   <si>
     <t>DZ,Medium,Play</t>
+  </si>
+  <si>
+    <t>Direct,Play</t>
+  </si>
+  <si>
+    <t>Direct,Medium,Play</t>
+  </si>
+  <si>
+    <t>Goal,not_one_timer,On_Net,OZ</t>
+  </si>
+  <si>
+    <t>Direct,OZ2,Play</t>
+  </si>
+  <si>
+    <t>Goal,no_traffic,On_Net,OZ,Short</t>
+  </si>
+  <si>
+    <t>Goal,On_Net,OZ</t>
+  </si>
+  <si>
+    <t>Direct,lfw,Play</t>
+  </si>
+  <si>
+    <t>Ang(N),Goal,not_one_timer,On_Net,OZ</t>
+  </si>
+  <si>
+    <t>Ang(N),Goal,On_Net,OZ</t>
+  </si>
+  <si>
+    <t>Medium,NZ2,Play</t>
+  </si>
+  <si>
+    <t>Indirect,Medium,Play</t>
+  </si>
+  <si>
+    <t>lfw,OZ,Play</t>
+  </si>
+  <si>
+    <t>lfw,Long,Play</t>
+  </si>
+  <si>
+    <t>OZ2,Play,Short</t>
+  </si>
+  <si>
+    <t>Direct,OZ2,Play,Short</t>
+  </si>
+  <si>
+    <t>Goal,no_traffic,On_Net,one_timer,OZ,Short,Snapshot</t>
+  </si>
+  <si>
+    <t>OZ,OZ2,Play,bw</t>
+  </si>
+  <si>
+    <t>OZ2,Play,bw</t>
+  </si>
+  <si>
+    <t>OZ,Play,bw</t>
+  </si>
+  <si>
+    <t>Goal,no_traffic,On_Net,OZ,Short,Snapshot</t>
+  </si>
+  <si>
+    <t>Direct,OZ2,Play,bw</t>
+  </si>
+  <si>
+    <t>Direct,Play,Short</t>
+  </si>
+  <si>
+    <t>Direct,OZ,OZ2,Play</t>
+  </si>
+  <si>
+    <t>Direct,OZ,Play</t>
+  </si>
+  <si>
+    <t>Direct,Play,bw</t>
+  </si>
+  <si>
+    <t>Direct,Play,Short,bw</t>
+  </si>
+  <si>
+    <t>Play,Short,bw</t>
   </si>
 </sst>
 </file>
@@ -598,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55971CB-5DFE-4FF4-BB31-EF2E4D53BB35}">
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="69" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:H2"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -607,8 +691,8 @@
     <col min="1" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -630,7 +714,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -647,7 +731,7 @@
       <c r="F2" s="2">
         <v>0.24196597353497201</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>0.92086330935251803</v>
       </c>
       <c r="H2" s="1">
@@ -667,7 +751,7 @@
       <c r="F3" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0.89230769230769202</v>
       </c>
       <c r="H3" s="1">
@@ -684,7 +768,7 @@
       <c r="F4" s="2">
         <v>0.12098298676748601</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>0.88888888888888895</v>
       </c>
       <c r="H4" s="1">
@@ -701,7 +785,7 @@
       <c r="F5" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>0.88524590163934402</v>
       </c>
       <c r="H5" s="1">
@@ -721,7 +805,7 @@
       <c r="F6" s="2">
         <v>0.128544423440454</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.87179487179487203</v>
       </c>
       <c r="H6" s="1">
@@ -738,7 +822,7 @@
       <c r="F7" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>0.88524590163934402</v>
       </c>
       <c r="H7" s="1">
@@ -755,7 +839,7 @@
       <c r="F8" s="2">
         <v>0.141776937618147</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>0.85227272727272696</v>
       </c>
       <c r="H8" s="1">
@@ -775,7 +859,7 @@
       <c r="F9" s="2">
         <v>0.103969754253308</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>0.84615384615384603</v>
       </c>
       <c r="H9" s="1">
@@ -792,7 +876,7 @@
       <c r="F10" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>0.87323943661971803</v>
       </c>
       <c r="H10" s="1">
@@ -812,7 +896,7 @@
       <c r="F11" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>0.86567164179104505</v>
       </c>
       <c r="H11" s="1">
@@ -832,7 +916,7 @@
       <c r="F12" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>0.82352941176470595</v>
       </c>
       <c r="H12" s="1">
@@ -849,7 +933,7 @@
       <c r="F13" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>0.81944444444444398</v>
       </c>
       <c r="H13" s="1">
@@ -866,7 +950,7 @@
       <c r="F14" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>0.84722222222222199</v>
       </c>
       <c r="H14" s="1">
@@ -883,7 +967,7 @@
       <c r="F15" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>0.81690140845070403</v>
       </c>
       <c r="H15" s="1">
@@ -900,7 +984,7 @@
       <c r="F16" s="2">
         <v>0.13988657844990501</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>0.84090909090909105</v>
       </c>
       <c r="H16" s="1">
@@ -920,7 +1004,7 @@
       <c r="F17" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>0.84057971014492805</v>
       </c>
       <c r="H17" s="1">
@@ -937,7 +1021,7 @@
       <c r="F18" s="2">
         <v>0.14744801512287301</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>0.83870967741935498</v>
       </c>
       <c r="H18" s="1">
@@ -954,7 +1038,7 @@
       <c r="F19" s="2">
         <v>0.141776937618147</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>0.80645161290322598</v>
       </c>
       <c r="H19" s="1">
@@ -974,7 +1058,7 @@
       <c r="F20" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>0.80597014925373101</v>
       </c>
       <c r="H20" s="1">
@@ -994,7 +1078,7 @@
       <c r="F21" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>0.83333333333333304</v>
       </c>
       <c r="H21" s="1">
@@ -1014,7 +1098,7 @@
       <c r="F22" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>0.83076923076923104</v>
       </c>
       <c r="H22" s="1">
@@ -1037,7 +1121,7 @@
       <c r="F23" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>0.828125</v>
       </c>
       <c r="H23" s="1">
@@ -1057,7 +1141,7 @@
       <c r="F24" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>0.82352941176470595</v>
       </c>
       <c r="H24" s="1">
@@ -1074,7 +1158,7 @@
       <c r="F25" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>0.81944444444444398</v>
       </c>
       <c r="H25" s="1">
@@ -1091,7 +1175,7 @@
       <c r="F26" s="2">
         <v>0.13610586011342199</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>0.81818181818181801</v>
       </c>
       <c r="H26" s="1">
@@ -1111,7 +1195,7 @@
       <c r="F27" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>0.81538461538461504</v>
       </c>
       <c r="H27" s="1">
@@ -1131,7 +1215,7 @@
       <c r="F28" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>0.8125</v>
       </c>
       <c r="H28" s="1">
@@ -1148,7 +1232,7 @@
       <c r="F29" s="2">
         <v>0.10775047258979201</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>0.80281690140845097</v>
       </c>
       <c r="H29" s="1">
@@ -1165,7 +1249,7 @@
       <c r="F30" s="2">
         <v>0.90548204158790202</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>1</v>
       </c>
       <c r="H30" s="1">
@@ -1182,7 +1266,7 @@
       <c r="F31" s="2">
         <v>0.48204158790170099</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>1</v>
       </c>
       <c r="H31" s="1">
@@ -1202,7 +1286,7 @@
       <c r="F32" s="2">
         <v>0.43856332703213602</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>1</v>
       </c>
       <c r="H32" s="1">
@@ -1219,7 +1303,7 @@
       <c r="F33" s="2">
         <v>0.35160680529300598</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
         <v>1</v>
       </c>
       <c r="H33" s="1">
@@ -1239,7 +1323,7 @@
       <c r="F34" s="2">
         <v>0.32136105860113401</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>1</v>
       </c>
       <c r="H34" s="1">
@@ -1256,7 +1340,7 @@
       <c r="F35" s="2">
         <v>0.27977315689981103</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="1">
         <v>1</v>
       </c>
       <c r="H35" s="1">
@@ -1273,7 +1357,7 @@
       <c r="F36" s="2">
         <v>0.27410207939508502</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="1">
         <v>1</v>
       </c>
       <c r="H36" s="1">
@@ -1290,7 +1374,7 @@
       <c r="F37" s="2">
         <v>0.262759924385633</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="1">
         <v>1</v>
       </c>
       <c r="H37" s="1">
@@ -1307,7 +1391,7 @@
       <c r="F38" s="2">
         <v>0.262759924385633</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
         <v>1</v>
       </c>
       <c r="H38" s="1">
@@ -1327,7 +1411,7 @@
       <c r="F39" s="2">
         <v>0.25141776937618099</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>1</v>
       </c>
       <c r="H39" s="1">
@@ -1344,7 +1428,7 @@
       <c r="F40" s="2">
         <v>0.24763705103969799</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
         <v>1</v>
       </c>
       <c r="H40" s="1">
@@ -1364,7 +1448,7 @@
       <c r="F41" s="2">
         <v>0.243856332703214</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>1</v>
       </c>
       <c r="H41" s="1">
@@ -1381,7 +1465,7 @@
       <c r="F42" s="2">
         <v>0.24196597353497201</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>1</v>
       </c>
       <c r="H42" s="1">
@@ -1398,7 +1482,7 @@
       <c r="F43" s="2">
         <v>0.23440453686200399</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>1</v>
       </c>
       <c r="H43" s="1">
@@ -1418,7 +1502,7 @@
       <c r="F44" s="2">
         <v>0.23251417769376201</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
         <v>1</v>
       </c>
       <c r="H44" s="1">
@@ -1435,7 +1519,7 @@
       <c r="F45" s="2">
         <v>0.23251417769376201</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>1</v>
       </c>
       <c r="H45" s="1">
@@ -1452,7 +1536,7 @@
       <c r="F46" s="2">
         <v>0.23062381852552</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
         <v>1</v>
       </c>
       <c r="H46" s="1">
@@ -1472,7 +1556,7 @@
       <c r="F47" s="2">
         <v>0.22117202268430999</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
         <v>1</v>
       </c>
       <c r="H47" s="1">
@@ -1492,7 +1576,7 @@
       <c r="F48" s="2">
         <v>0.22117202268430999</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
         <v>1</v>
       </c>
       <c r="H48" s="1">
@@ -1509,7 +1593,7 @@
       <c r="F49" s="2">
         <v>0.21928166351606801</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="1">
         <v>1</v>
       </c>
       <c r="H49" s="1">
@@ -1526,7 +1610,7 @@
       <c r="F50" s="2">
         <v>0.21928166351606801</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="1">
         <v>1</v>
       </c>
       <c r="H50" s="1">
@@ -1546,7 +1630,7 @@
       <c r="F51" s="2">
         <v>0.21928166351606801</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="1">
         <v>1</v>
       </c>
       <c r="H51" s="1">
@@ -1569,7 +1653,7 @@
       <c r="F52" s="2">
         <v>0.217391304347826</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="1">
         <v>1</v>
       </c>
       <c r="H52" s="1">
@@ -1589,7 +1673,7 @@
       <c r="F53" s="2">
         <v>0.213610586011342</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="1">
         <v>1</v>
       </c>
       <c r="H53" s="1">
@@ -1609,7 +1693,7 @@
       <c r="F54" s="2">
         <v>0.21172022684309999</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54" s="1">
         <v>1</v>
       </c>
       <c r="H54" s="1">
@@ -1629,7 +1713,7 @@
       <c r="F55" s="2">
         <v>0.194706994328922</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="1">
         <v>1</v>
       </c>
       <c r="H55" s="1">
@@ -1646,7 +1730,7 @@
       <c r="F56" s="2">
         <v>0.177693761814745</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="1">
         <v>1</v>
       </c>
       <c r="H56" s="1">
@@ -1663,7 +1747,7 @@
       <c r="F57" s="2">
         <v>0.177693761814745</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="1">
         <v>1</v>
       </c>
       <c r="H57" s="1">
@@ -1680,7 +1764,7 @@
       <c r="F58" s="2">
         <v>0.17580340264650299</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58" s="1">
         <v>1</v>
       </c>
       <c r="H58" s="1">
@@ -1697,7 +1781,7 @@
       <c r="F59" s="2">
         <v>0.17202268431001899</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59" s="1">
         <v>1</v>
       </c>
       <c r="H59" s="1">
@@ -1717,7 +1801,7 @@
       <c r="F60" s="2">
         <v>0.17202268431001899</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="1">
         <v>1</v>
       </c>
       <c r="H60" s="1">
@@ -1737,7 +1821,7 @@
       <c r="F61" s="2">
         <v>0.168241965973535</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="1">
         <v>1</v>
       </c>
       <c r="H61" s="1">
@@ -1754,7 +1838,7 @@
       <c r="F62" s="2">
         <v>0.168241965973535</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="1">
         <v>1</v>
       </c>
       <c r="H62" s="1">
@@ -1771,7 +1855,7 @@
       <c r="F63" s="2">
         <v>0.168241965973535</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
         <v>1</v>
       </c>
       <c r="H63" s="1">
@@ -1788,7 +1872,7 @@
       <c r="F64" s="2">
         <v>0.16635160680529301</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
         <v>1</v>
       </c>
       <c r="H64" s="1">
@@ -1805,7 +1889,7 @@
       <c r="F65" s="2">
         <v>0.16635160680529301</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
         <v>1</v>
       </c>
       <c r="H65" s="1">
@@ -1825,7 +1909,7 @@
       <c r="F66" s="2">
         <v>0.164461247637051</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
         <v>1</v>
       </c>
       <c r="H66" s="1">
@@ -1848,7 +1932,7 @@
       <c r="F67" s="2">
         <v>0.164461247637051</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="1">
         <v>1</v>
       </c>
       <c r="H67" s="1">
@@ -1868,7 +1952,7 @@
       <c r="F68" s="2">
         <v>0.160680529300567</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
         <v>1</v>
       </c>
       <c r="H68" s="1">
@@ -1888,7 +1972,7 @@
       <c r="F69" s="2">
         <v>0.15879017013232499</v>
       </c>
-      <c r="G69" s="2">
+      <c r="G69" s="1">
         <v>1</v>
       </c>
       <c r="H69" s="1">
@@ -1905,7 +1989,7 @@
       <c r="F70" s="2">
         <v>0.15879017013232499</v>
       </c>
-      <c r="G70" s="2">
+      <c r="G70" s="1">
         <v>1</v>
       </c>
       <c r="H70" s="1">
@@ -1925,7 +2009,7 @@
       <c r="F71" s="2">
         <v>0.15689981096408301</v>
       </c>
-      <c r="G71" s="2">
+      <c r="G71" s="1">
         <v>1</v>
       </c>
       <c r="H71" s="1">
@@ -1948,7 +2032,7 @@
       <c r="F72" s="2">
         <v>0.15689981096408301</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="1">
         <v>1</v>
       </c>
       <c r="H72" s="1">
@@ -1968,7 +2052,7 @@
       <c r="F73" s="2">
         <v>0.15689981096408301</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73" s="1">
         <v>1</v>
       </c>
       <c r="H73" s="1">
@@ -1988,7 +2072,7 @@
       <c r="F74" s="2">
         <v>0.15311909262759901</v>
       </c>
-      <c r="G74" s="2">
+      <c r="G74" s="1">
         <v>1</v>
       </c>
       <c r="H74" s="1">
@@ -2008,7 +2092,7 @@
       <c r="F75" s="2">
         <v>0.151228733459357</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75" s="1">
         <v>1</v>
       </c>
       <c r="H75" s="1">
@@ -2025,7 +2109,7 @@
       <c r="F76" s="2">
         <v>0.151228733459357</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G76" s="1">
         <v>1</v>
       </c>
       <c r="H76" s="1">
@@ -2042,7 +2126,7 @@
       <c r="F77" s="2">
         <v>0.14744801512287301</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77" s="1">
         <v>1</v>
       </c>
       <c r="H77" s="1">
@@ -2062,7 +2146,7 @@
       <c r="F78" s="2">
         <v>0.14744801512287301</v>
       </c>
-      <c r="G78" s="2">
+      <c r="G78" s="1">
         <v>1</v>
       </c>
       <c r="H78" s="1">
@@ -2079,7 +2163,7 @@
       <c r="F79" s="2">
         <v>0.141776937618147</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79" s="1">
         <v>1</v>
       </c>
       <c r="H79" s="1">
@@ -2099,7 +2183,7 @@
       <c r="F80" s="2">
         <v>0.141776937618147</v>
       </c>
-      <c r="G80" s="2">
+      <c r="G80" s="1">
         <v>1</v>
       </c>
       <c r="H80" s="1">
@@ -2116,7 +2200,7 @@
       <c r="F81" s="2">
         <v>0.13988657844990501</v>
       </c>
-      <c r="G81" s="2">
+      <c r="G81" s="1">
         <v>1</v>
       </c>
       <c r="H81" s="1">
@@ -2133,7 +2217,7 @@
       <c r="F82" s="2">
         <v>0.13610586011342199</v>
       </c>
-      <c r="G82" s="2">
+      <c r="G82" s="1">
         <v>1</v>
       </c>
       <c r="H82" s="1">
@@ -2150,7 +2234,7 @@
       <c r="F83" s="2">
         <v>0.13610586011342199</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G83" s="1">
         <v>1</v>
       </c>
       <c r="H83" s="1">
@@ -2167,7 +2251,7 @@
       <c r="F84" s="2">
         <v>0.13421550094518001</v>
       </c>
-      <c r="G84" s="2">
+      <c r="G84" s="1">
         <v>1</v>
       </c>
       <c r="H84" s="1">
@@ -2187,7 +2271,7 @@
       <c r="F85" s="2">
         <v>0.13421550094518001</v>
       </c>
-      <c r="G85" s="2">
+      <c r="G85" s="1">
         <v>1</v>
       </c>
       <c r="H85" s="1">
@@ -2207,7 +2291,7 @@
       <c r="F86" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G86" s="2">
+      <c r="G86" s="1">
         <v>1</v>
       </c>
       <c r="H86" s="1">
@@ -2227,7 +2311,7 @@
       <c r="F87" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G87" s="2">
+      <c r="G87" s="1">
         <v>1</v>
       </c>
       <c r="H87" s="1">
@@ -2247,7 +2331,7 @@
       <c r="F88" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G88" s="1">
         <v>1</v>
       </c>
       <c r="H88" s="1">
@@ -2267,7 +2351,7 @@
       <c r="F89" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G89" s="2">
+      <c r="G89" s="1">
         <v>1</v>
       </c>
       <c r="H89" s="1">
@@ -2284,7 +2368,7 @@
       <c r="F90" s="2">
         <v>0.13232514177693799</v>
       </c>
-      <c r="G90" s="2">
+      <c r="G90" s="1">
         <v>1</v>
       </c>
       <c r="H90" s="1">
@@ -2304,7 +2388,7 @@
       <c r="F91" s="2">
         <v>0.13043478260869601</v>
       </c>
-      <c r="G91" s="2">
+      <c r="G91" s="1">
         <v>1</v>
       </c>
       <c r="H91" s="1">
@@ -2321,7 +2405,7 @@
       <c r="F92" s="2">
         <v>0.13043478260869601</v>
       </c>
-      <c r="G92" s="2">
+      <c r="G92" s="1">
         <v>1</v>
       </c>
       <c r="H92" s="1">
@@ -2341,7 +2425,7 @@
       <c r="F93" s="2">
         <v>0.13043478260869601</v>
       </c>
-      <c r="G93" s="2">
+      <c r="G93" s="1">
         <v>1</v>
       </c>
       <c r="H93" s="1">
@@ -2361,7 +2445,7 @@
       <c r="F94" s="2">
         <v>0.13043478260869601</v>
       </c>
-      <c r="G94" s="2">
+      <c r="G94" s="1">
         <v>1</v>
       </c>
       <c r="H94" s="1">
@@ -2381,7 +2465,7 @@
       <c r="F95" s="2">
         <v>0.128544423440454</v>
       </c>
-      <c r="G95" s="2">
+      <c r="G95" s="1">
         <v>1</v>
       </c>
       <c r="H95" s="1">
@@ -2401,7 +2485,7 @@
       <c r="F96" s="2">
         <v>0.128544423440454</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G96" s="1">
         <v>1</v>
       </c>
       <c r="H96" s="1">
@@ -2421,7 +2505,7 @@
       <c r="F97" s="2">
         <v>0.12665406427221201</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G97" s="1">
         <v>1</v>
       </c>
       <c r="H97" s="1">
@@ -2438,7 +2522,7 @@
       <c r="F98" s="2">
         <v>0.12665406427221201</v>
       </c>
-      <c r="G98" s="2">
+      <c r="G98" s="1">
         <v>1</v>
       </c>
       <c r="H98" s="1">
@@ -2458,7 +2542,7 @@
       <c r="F99" s="2">
         <v>0.12665406427221201</v>
       </c>
-      <c r="G99" s="2">
+      <c r="G99" s="1">
         <v>1</v>
       </c>
       <c r="H99" s="1">
@@ -2475,7 +2559,7 @@
       <c r="F100" s="2">
         <v>0.12476370510397</v>
       </c>
-      <c r="G100" s="2">
+      <c r="G100" s="1">
         <v>1</v>
       </c>
       <c r="H100" s="1">
@@ -2498,7 +2582,7 @@
       <c r="F101" s="2">
         <v>0.12476370510397</v>
       </c>
-      <c r="G101" s="2">
+      <c r="G101" s="1">
         <v>1</v>
       </c>
       <c r="H101" s="1">
@@ -2518,7 +2602,7 @@
       <c r="F102" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G102" s="2">
+      <c r="G102" s="1">
         <v>1</v>
       </c>
       <c r="H102" s="1">
@@ -2541,7 +2625,7 @@
       <c r="F103" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G103" s="2">
+      <c r="G103" s="1">
         <v>1</v>
       </c>
       <c r="H103" s="1">
@@ -2561,7 +2645,7 @@
       <c r="F104" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G104" s="2">
+      <c r="G104" s="1">
         <v>1</v>
       </c>
       <c r="H104" s="1">
@@ -2581,7 +2665,7 @@
       <c r="F105" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G105" s="2">
+      <c r="G105" s="1">
         <v>1</v>
       </c>
       <c r="H105" s="1">
@@ -2604,7 +2688,7 @@
       <c r="F106" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G106" s="2">
+      <c r="G106" s="1">
         <v>1</v>
       </c>
       <c r="H106" s="1">
@@ -2624,7 +2708,7 @@
       <c r="F107" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G107" s="2">
+      <c r="G107" s="1">
         <v>1</v>
       </c>
       <c r="H107" s="1">
@@ -2647,7 +2731,7 @@
       <c r="F108" s="2">
         <v>0.122873345935728</v>
       </c>
-      <c r="G108" s="2">
+      <c r="G108" s="1">
         <v>1</v>
       </c>
       <c r="H108" s="1">
@@ -2670,7 +2754,7 @@
       <c r="F109" s="2">
         <v>0.12098298676748601</v>
       </c>
-      <c r="G109" s="2">
+      <c r="G109" s="1">
         <v>1</v>
       </c>
       <c r="H109" s="1">
@@ -2687,7 +2771,7 @@
       <c r="F110" s="2">
         <v>0.12098298676748601</v>
       </c>
-      <c r="G110" s="2">
+      <c r="G110" s="1">
         <v>1</v>
       </c>
       <c r="H110" s="1">
@@ -2704,7 +2788,7 @@
       <c r="F111" s="2">
         <v>0.12098298676748601</v>
       </c>
-      <c r="G111" s="2">
+      <c r="G111" s="1">
         <v>1</v>
       </c>
       <c r="H111" s="1">
@@ -2727,7 +2811,7 @@
       <c r="F112" s="2">
         <v>0.12098298676748601</v>
       </c>
-      <c r="G112" s="2">
+      <c r="G112" s="1">
         <v>1</v>
       </c>
       <c r="H112" s="1">
@@ -2747,7 +2831,7 @@
       <c r="F113" s="2">
         <v>0.11909262759924399</v>
       </c>
-      <c r="G113" s="2">
+      <c r="G113" s="1">
         <v>1</v>
       </c>
       <c r="H113" s="1">
@@ -2767,7 +2851,7 @@
       <c r="F114" s="2">
         <v>0.11909262759924399</v>
       </c>
-      <c r="G114" s="2">
+      <c r="G114" s="1">
         <v>1</v>
       </c>
       <c r="H114" s="1">
@@ -2787,7 +2871,7 @@
       <c r="F115" s="2">
         <v>0.11909262759924399</v>
       </c>
-      <c r="G115" s="2">
+      <c r="G115" s="1">
         <v>1</v>
       </c>
       <c r="H115" s="1">
@@ -2807,7 +2891,7 @@
       <c r="F116" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G116" s="2">
+      <c r="G116" s="1">
         <v>1</v>
       </c>
       <c r="H116" s="1">
@@ -2827,7 +2911,7 @@
       <c r="F117" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G117" s="2">
+      <c r="G117" s="1">
         <v>1</v>
       </c>
       <c r="H117" s="1">
@@ -2853,7 +2937,7 @@
       <c r="F118" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G118" s="2">
+      <c r="G118" s="1">
         <v>1</v>
       </c>
       <c r="H118" s="1">
@@ -2870,7 +2954,7 @@
       <c r="F119" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G119" s="2">
+      <c r="G119" s="1">
         <v>1</v>
       </c>
       <c r="H119" s="1">
@@ -2890,7 +2974,7 @@
       <c r="F120" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G120" s="2">
+      <c r="G120" s="1">
         <v>1</v>
       </c>
       <c r="H120" s="1">
@@ -2910,7 +2994,7 @@
       <c r="F121" s="2">
         <v>0.117202268431002</v>
       </c>
-      <c r="G121" s="2">
+      <c r="G121" s="1">
         <v>1</v>
       </c>
       <c r="H121" s="1">
@@ -2930,7 +3014,7 @@
       <c r="F122" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G122" s="2">
+      <c r="G122" s="1">
         <v>1</v>
       </c>
       <c r="H122" s="1">
@@ -2947,7 +3031,7 @@
       <c r="F123" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G123" s="2">
+      <c r="G123" s="1">
         <v>1</v>
       </c>
       <c r="H123" s="1">
@@ -2967,7 +3051,7 @@
       <c r="F124" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G124" s="2">
+      <c r="G124" s="1">
         <v>1</v>
       </c>
       <c r="H124" s="1">
@@ -2984,7 +3068,7 @@
       <c r="F125" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G125" s="2">
+      <c r="G125" s="1">
         <v>1</v>
       </c>
       <c r="H125" s="1">
@@ -3007,7 +3091,7 @@
       <c r="F126" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G126" s="2">
+      <c r="G126" s="1">
         <v>1</v>
       </c>
       <c r="H126" s="1">
@@ -3024,7 +3108,7 @@
       <c r="F127" s="2">
         <v>0.11531190926276</v>
       </c>
-      <c r="G127" s="2">
+      <c r="G127" s="1">
         <v>1</v>
       </c>
       <c r="H127" s="1">
@@ -3047,7 +3131,7 @@
       <c r="F128" s="2">
         <v>0.113421550094518</v>
       </c>
-      <c r="G128" s="2">
+      <c r="G128" s="1">
         <v>1</v>
       </c>
       <c r="H128" s="1">
@@ -3067,7 +3151,7 @@
       <c r="F129" s="2">
         <v>0.113421550094518</v>
       </c>
-      <c r="G129" s="2">
+      <c r="G129" s="1">
         <v>1</v>
       </c>
       <c r="H129" s="1">
@@ -3090,7 +3174,7 @@
       <c r="F130" s="2">
         <v>0.113421550094518</v>
       </c>
-      <c r="G130" s="2">
+      <c r="G130" s="1">
         <v>1</v>
       </c>
       <c r="H130" s="1">
@@ -3110,7 +3194,7 @@
       <c r="F131" s="2">
         <v>0.113421550094518</v>
       </c>
-      <c r="G131" s="2">
+      <c r="G131" s="1">
         <v>1</v>
       </c>
       <c r="H131" s="1">
@@ -3133,7 +3217,7 @@
       <c r="F132" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G132" s="2">
+      <c r="G132" s="1">
         <v>1</v>
       </c>
       <c r="H132" s="1">
@@ -3153,7 +3237,7 @@
       <c r="F133" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G133" s="2">
+      <c r="G133" s="1">
         <v>1</v>
       </c>
       <c r="H133" s="1">
@@ -3176,7 +3260,7 @@
       <c r="F134" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G134" s="2">
+      <c r="G134" s="1">
         <v>1</v>
       </c>
       <c r="H134" s="1">
@@ -3196,7 +3280,7 @@
       <c r="F135" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G135" s="2">
+      <c r="G135" s="1">
         <v>1</v>
       </c>
       <c r="H135" s="1">
@@ -3213,7 +3297,7 @@
       <c r="F136" s="2">
         <v>0.111531190926276</v>
       </c>
-      <c r="G136" s="2">
+      <c r="G136" s="1">
         <v>1</v>
       </c>
       <c r="H136" s="1">
@@ -3233,7 +3317,7 @@
       <c r="F137" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G137" s="2">
+      <c r="G137" s="1">
         <v>1</v>
       </c>
       <c r="H137" s="1">
@@ -3253,7 +3337,7 @@
       <c r="F138" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G138" s="2">
+      <c r="G138" s="1">
         <v>1</v>
       </c>
       <c r="H138" s="1">
@@ -3273,7 +3357,7 @@
       <c r="F139" s="2">
         <v>0.109640831758034</v>
       </c>
-      <c r="G139" s="2">
+      <c r="G139" s="1">
         <v>1</v>
       </c>
       <c r="H139" s="1">
@@ -3293,7 +3377,7 @@
       <c r="F140" s="2">
         <v>0.10775047258979201</v>
       </c>
-      <c r="G140" s="2">
+      <c r="G140" s="1">
         <v>1</v>
       </c>
       <c r="H140" s="1">
@@ -3310,7 +3394,7 @@
       <c r="F141" s="2">
         <v>0.10775047258979201</v>
       </c>
-      <c r="G141" s="2">
+      <c r="G141" s="1">
         <v>1</v>
       </c>
       <c r="H141" s="1">
@@ -3327,7 +3411,7 @@
       <c r="F142" s="2">
         <v>0.10775047258979201</v>
       </c>
-      <c r="G142" s="2">
+      <c r="G142" s="1">
         <v>1</v>
       </c>
       <c r="H142" s="1">
@@ -3347,7 +3431,7 @@
       <c r="F143" s="2">
         <v>0.10586011342155</v>
       </c>
-      <c r="G143" s="2">
+      <c r="G143" s="1">
         <v>1</v>
       </c>
       <c r="H143" s="1">
@@ -3370,7 +3454,7 @@
       <c r="F144" s="2">
         <v>0.10586011342155</v>
       </c>
-      <c r="G144" s="2">
+      <c r="G144" s="1">
         <v>1</v>
       </c>
       <c r="H144" s="1">
@@ -3387,7 +3471,7 @@
       <c r="F145" s="2">
         <v>0.10586011342155</v>
       </c>
-      <c r="G145" s="2">
+      <c r="G145" s="1">
         <v>1</v>
       </c>
       <c r="H145" s="1">
@@ -3404,7 +3488,7 @@
       <c r="F146" s="2">
         <v>0.10586011342155</v>
       </c>
-      <c r="G146" s="2">
+      <c r="G146" s="1">
         <v>1</v>
       </c>
       <c r="H146" s="1">
@@ -3424,7 +3508,7 @@
       <c r="F147" s="2">
         <v>0.10586011342155</v>
       </c>
-      <c r="G147" s="2">
+      <c r="G147" s="1">
         <v>1</v>
       </c>
       <c r="H147" s="1">
@@ -3444,7 +3528,7 @@
       <c r="F148" s="2">
         <v>0.10586011342155</v>
       </c>
-      <c r="G148" s="2">
+      <c r="G148" s="1">
         <v>1</v>
       </c>
       <c r="H148" s="1">
@@ -3461,7 +3545,7 @@
       <c r="F149" s="2">
         <v>0.103969754253308</v>
       </c>
-      <c r="G149" s="2">
+      <c r="G149" s="1">
         <v>1</v>
       </c>
       <c r="H149" s="1">
@@ -3478,7 +3562,7 @@
       <c r="F150" s="2">
         <v>0.103969754253308</v>
       </c>
-      <c r="G150" s="2">
+      <c r="G150" s="1">
         <v>1</v>
       </c>
       <c r="H150" s="1">
@@ -3498,7 +3582,7 @@
       <c r="F151" s="2">
         <v>0.103969754253308</v>
       </c>
-      <c r="G151" s="2">
+      <c r="G151" s="1">
         <v>1</v>
       </c>
       <c r="H151" s="1">
@@ -3521,7 +3605,7 @@
       <c r="F152" s="2">
         <v>0.103969754253308</v>
       </c>
-      <c r="G152" s="2">
+      <c r="G152" s="1">
         <v>1</v>
       </c>
       <c r="H152" s="1">
@@ -3541,7 +3625,7 @@
       <c r="F153" s="2">
         <v>0.103969754253308</v>
       </c>
-      <c r="G153" s="2">
+      <c r="G153" s="1">
         <v>1</v>
       </c>
       <c r="H153" s="1">
@@ -3561,7 +3645,7 @@
       <c r="F154" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G154" s="2">
+      <c r="G154" s="1">
         <v>1</v>
       </c>
       <c r="H154" s="1">
@@ -3581,7 +3665,7 @@
       <c r="F155" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G155" s="2">
+      <c r="G155" s="1">
         <v>1</v>
       </c>
       <c r="H155" s="1">
@@ -3601,7 +3685,7 @@
       <c r="F156" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G156" s="2">
+      <c r="G156" s="1">
         <v>1</v>
       </c>
       <c r="H156" s="1">
@@ -3624,7 +3708,7 @@
       <c r="F157" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G157" s="2">
+      <c r="G157" s="1">
         <v>1</v>
       </c>
       <c r="H157" s="1">
@@ -3644,7 +3728,7 @@
       <c r="F158" s="2">
         <v>0.102079395085066</v>
       </c>
-      <c r="G158" s="2">
+      <c r="G158" s="1">
         <v>1</v>
       </c>
       <c r="H158" s="1">
@@ -3667,7 +3751,7 @@
       <c r="F159" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G159" s="2">
+      <c r="G159" s="1">
         <v>1</v>
       </c>
       <c r="H159" s="1">
@@ -3687,7 +3771,7 @@
       <c r="F160" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G160" s="2">
+      <c r="G160" s="1">
         <v>1</v>
       </c>
       <c r="H160" s="1">
@@ -3710,7 +3794,7 @@
       <c r="F161" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G161" s="2">
+      <c r="G161" s="1">
         <v>1</v>
       </c>
       <c r="H161" s="1">
@@ -3730,7 +3814,7 @@
       <c r="F162" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G162" s="2">
+      <c r="G162" s="1">
         <v>1</v>
       </c>
       <c r="H162" s="1">
@@ -3747,7 +3831,7 @@
       <c r="F163" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G163" s="2">
+      <c r="G163" s="1">
         <v>1</v>
       </c>
       <c r="H163" s="1">
@@ -3767,7 +3851,7 @@
       <c r="F164" s="2">
         <v>0.100189035916824</v>
       </c>
-      <c r="G164" s="2">
+      <c r="G164" s="1">
         <v>1</v>
       </c>
       <c r="H164" s="1">
@@ -3778,4 +3862,2861 @@
   <autoFilter ref="A1:H164" xr:uid="{C55971CB-5DFE-4FF4-BB31-EF2E4D53BB35}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1CE54B-C390-4F18-ADA1-28618FC01C70}">
+  <dimension ref="A1:H127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="2"/>
+    <col min="7" max="8" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1.28571428571429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1.0714285714285701</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1.0714285714285701</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1.0714285714285701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+      <c r="H48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" t="s">
+        <v>65</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>65</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>65</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>65</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>65</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" t="s">
+        <v>65</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" t="s">
+        <v>65</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" t="s">
+        <v>65</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" t="s">
+        <v>65</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" t="s">
+        <v>23</v>
+      </c>
+      <c r="E64" t="s">
+        <v>65</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s">
+        <v>65</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" t="s">
+        <v>65</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>65</v>
+      </c>
+      <c r="F67" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>65</v>
+      </c>
+      <c r="F68" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" t="s">
+        <v>65</v>
+      </c>
+      <c r="F70" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>65</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>65</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>65</v>
+      </c>
+      <c r="F73" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" t="s">
+        <v>65</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" t="s">
+        <v>65</v>
+      </c>
+      <c r="F75" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G75" s="1">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" t="s">
+        <v>65</v>
+      </c>
+      <c r="F76" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" t="s">
+        <v>63</v>
+      </c>
+      <c r="E77" t="s">
+        <v>65</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>63</v>
+      </c>
+      <c r="E78" t="s">
+        <v>65</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79" t="s">
+        <v>65</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1</v>
+      </c>
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E80" t="s">
+        <v>65</v>
+      </c>
+      <c r="F80" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+      <c r="H80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" t="s">
+        <v>31</v>
+      </c>
+      <c r="E81" t="s">
+        <v>65</v>
+      </c>
+      <c r="F81" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G81" s="1">
+        <v>1</v>
+      </c>
+      <c r="H81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>72</v>
+      </c>
+      <c r="E82" t="s">
+        <v>65</v>
+      </c>
+      <c r="F82" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" t="s">
+        <v>72</v>
+      </c>
+      <c r="E83" t="s">
+        <v>65</v>
+      </c>
+      <c r="F83" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>65</v>
+      </c>
+      <c r="F84" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1</v>
+      </c>
+      <c r="H84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" t="s">
+        <v>65</v>
+      </c>
+      <c r="F85" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G85" s="1">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" t="s">
+        <v>65</v>
+      </c>
+      <c r="F86" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1</v>
+      </c>
+      <c r="H86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>66</v>
+      </c>
+      <c r="E87" t="s">
+        <v>65</v>
+      </c>
+      <c r="F87" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1</v>
+      </c>
+      <c r="H87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>66</v>
+      </c>
+      <c r="E88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F88" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G88" s="1">
+        <v>1</v>
+      </c>
+      <c r="H88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" t="s">
+        <v>60</v>
+      </c>
+      <c r="E89" t="s">
+        <v>65</v>
+      </c>
+      <c r="F89" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G89" s="1">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" t="s">
+        <v>70</v>
+      </c>
+      <c r="D90" t="s">
+        <v>60</v>
+      </c>
+      <c r="E90" t="s">
+        <v>65</v>
+      </c>
+      <c r="F90" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G90" s="1">
+        <v>1</v>
+      </c>
+      <c r="H90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" t="s">
+        <v>60</v>
+      </c>
+      <c r="E91" t="s">
+        <v>65</v>
+      </c>
+      <c r="F91" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G91" s="1">
+        <v>1</v>
+      </c>
+      <c r="H91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" t="s">
+        <v>43</v>
+      </c>
+      <c r="D92" t="s">
+        <v>60</v>
+      </c>
+      <c r="E92" t="s">
+        <v>65</v>
+      </c>
+      <c r="F92" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G92" s="1">
+        <v>1</v>
+      </c>
+      <c r="H92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>60</v>
+      </c>
+      <c r="E93" t="s">
+        <v>65</v>
+      </c>
+      <c r="F93" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G93" s="1">
+        <v>1</v>
+      </c>
+      <c r="H93" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>65</v>
+      </c>
+      <c r="F94" s="2">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="G94" s="1">
+        <v>1</v>
+      </c>
+      <c r="H94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" t="s">
+        <v>60</v>
+      </c>
+      <c r="E95" t="s">
+        <v>65</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="G95" s="1">
+        <v>1</v>
+      </c>
+      <c r="H95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" t="s">
+        <v>65</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="G96" s="1">
+        <v>1</v>
+      </c>
+      <c r="H96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" t="s">
+        <v>65</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="G97" s="1">
+        <v>1</v>
+      </c>
+      <c r="H97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E98" t="s">
+        <v>65</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G98" s="1">
+        <v>1</v>
+      </c>
+      <c r="H98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" t="s">
+        <v>81</v>
+      </c>
+      <c r="E99" t="s">
+        <v>65</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G99" s="1">
+        <v>1</v>
+      </c>
+      <c r="H99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" t="s">
+        <v>65</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G100" s="1">
+        <v>1</v>
+      </c>
+      <c r="H100" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>10</v>
+      </c>
+      <c r="D101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>65</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G101" s="1">
+        <v>1</v>
+      </c>
+      <c r="H101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" t="s">
+        <v>65</v>
+      </c>
+      <c r="F102" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G102" s="1">
+        <v>1</v>
+      </c>
+      <c r="H102" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103" t="s">
+        <v>65</v>
+      </c>
+      <c r="F103" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G103" s="1">
+        <v>1</v>
+      </c>
+      <c r="H103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104" t="s">
+        <v>18</v>
+      </c>
+      <c r="E104" t="s">
+        <v>65</v>
+      </c>
+      <c r="F104" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1</v>
+      </c>
+      <c r="H104" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" t="s">
+        <v>65</v>
+      </c>
+      <c r="F105" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G105" s="1">
+        <v>1</v>
+      </c>
+      <c r="H105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" t="s">
+        <v>82</v>
+      </c>
+      <c r="E106" t="s">
+        <v>65</v>
+      </c>
+      <c r="F106" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G106" s="1">
+        <v>1</v>
+      </c>
+      <c r="H106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" t="s">
+        <v>82</v>
+      </c>
+      <c r="E107" t="s">
+        <v>65</v>
+      </c>
+      <c r="F107" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G107" s="1">
+        <v>1</v>
+      </c>
+      <c r="H107" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108" t="s">
+        <v>63</v>
+      </c>
+      <c r="E108" t="s">
+        <v>65</v>
+      </c>
+      <c r="F108" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G108" s="1">
+        <v>1</v>
+      </c>
+      <c r="H108" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" t="s">
+        <v>77</v>
+      </c>
+      <c r="E109" t="s">
+        <v>65</v>
+      </c>
+      <c r="F109" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1</v>
+      </c>
+      <c r="H109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" t="s">
+        <v>65</v>
+      </c>
+      <c r="F110" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1</v>
+      </c>
+      <c r="H110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>83</v>
+      </c>
+      <c r="E111" t="s">
+        <v>65</v>
+      </c>
+      <c r="F111" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G111" s="1">
+        <v>1</v>
+      </c>
+      <c r="H111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" t="s">
+        <v>83</v>
+      </c>
+      <c r="E112" t="s">
+        <v>65</v>
+      </c>
+      <c r="F112" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1</v>
+      </c>
+      <c r="H112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" t="s">
+        <v>60</v>
+      </c>
+      <c r="E113" t="s">
+        <v>65</v>
+      </c>
+      <c r="F113" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G113" s="1">
+        <v>1</v>
+      </c>
+      <c r="H113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>84</v>
+      </c>
+      <c r="E114" t="s">
+        <v>65</v>
+      </c>
+      <c r="F114" s="2">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1</v>
+      </c>
+      <c r="H114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" t="s">
+        <v>73</v>
+      </c>
+      <c r="E115" t="s">
+        <v>65</v>
+      </c>
+      <c r="F115" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1</v>
+      </c>
+      <c r="H115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116" t="s">
+        <v>74</v>
+      </c>
+      <c r="E116" t="s">
+        <v>65</v>
+      </c>
+      <c r="F116" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G116" s="1">
+        <v>1</v>
+      </c>
+      <c r="H116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>85</v>
+      </c>
+      <c r="E117" t="s">
+        <v>65</v>
+      </c>
+      <c r="F117" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G117" s="1">
+        <v>1</v>
+      </c>
+      <c r="H117" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" t="s">
+        <v>86</v>
+      </c>
+      <c r="E118" t="s">
+        <v>65</v>
+      </c>
+      <c r="F118" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G118" s="1">
+        <v>1</v>
+      </c>
+      <c r="H118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" t="s">
+        <v>76</v>
+      </c>
+      <c r="E119" t="s">
+        <v>65</v>
+      </c>
+      <c r="F119" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G119" s="1">
+        <v>1</v>
+      </c>
+      <c r="H119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" t="s">
+        <v>76</v>
+      </c>
+      <c r="E120" t="s">
+        <v>65</v>
+      </c>
+      <c r="F120" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G120" s="1">
+        <v>1</v>
+      </c>
+      <c r="H120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121" t="s">
+        <v>80</v>
+      </c>
+      <c r="E121" t="s">
+        <v>65</v>
+      </c>
+      <c r="F121" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G121" s="1">
+        <v>1</v>
+      </c>
+      <c r="H121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" t="s">
+        <v>77</v>
+      </c>
+      <c r="E122" t="s">
+        <v>65</v>
+      </c>
+      <c r="F122" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G122" s="1">
+        <v>1</v>
+      </c>
+      <c r="H122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" t="s">
+        <v>78</v>
+      </c>
+      <c r="E123" t="s">
+        <v>65</v>
+      </c>
+      <c r="F123" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G123" s="1">
+        <v>1</v>
+      </c>
+      <c r="H123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124" t="s">
+        <v>78</v>
+      </c>
+      <c r="E124" t="s">
+        <v>65</v>
+      </c>
+      <c r="F124" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G124" s="1">
+        <v>1</v>
+      </c>
+      <c r="H124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" t="s">
+        <v>65</v>
+      </c>
+      <c r="F125" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G125" s="1">
+        <v>1</v>
+      </c>
+      <c r="H125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D126" t="s">
+        <v>10</v>
+      </c>
+      <c r="E126" t="s">
+        <v>65</v>
+      </c>
+      <c r="F126" s="2">
+        <v>1</v>
+      </c>
+      <c r="G126" s="1">
+        <v>1</v>
+      </c>
+      <c r="H126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D127" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" t="s">
+        <v>65</v>
+      </c>
+      <c r="F127" s="2">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="G127" s="1">
+        <v>1</v>
+      </c>
+      <c r="H127" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H127" xr:uid="{FA1CE54B-C390-4F18-ADA1-28618FC01C70}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H127">
+      <sortCondition descending="1" ref="H1:H127"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F83D001-EBFC-4C90-8CD4-BA87F5E7FBF1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>